<commit_message>
Minor changes to the file names, cleaned them up so that the specific filenames are correct...
</commit_message>
<xml_diff>
--- a/metadata/iReceptor_example_metadata_outline.xlsx
+++ b/metadata/iReceptor_example_metadata_outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcorrie\Documents\Source\dataloading-curation\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784929E6-A4F3-4290-B9D0-4D1FCC319FC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA808F2-27C4-4455-840F-555CD8A7E5BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{34AD7A3A-B4E1-4AE0-8A8A-2D7A7A71B3DB}"/>
+    <workbookView xWindow="33135" yWindow="2835" windowWidth="21225" windowHeight="11385" activeTab="1" xr2:uid="{34AD7A3A-B4E1-4AE0-8A8A-2D7A7A71B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="420">
   <si>
     <t>ir_record_number</t>
   </si>
@@ -619,27 +619,6 @@
     <t>VDJ</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">H.pylori </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>and unknown</t>
-    </r>
-  </si>
-  <si>
     <t>barcode, forward 11</t>
   </si>
   <si>
@@ -658,9 +637,6 @@
     <t>SRR873442_2_8.txz</t>
   </si>
   <si>
-    <t>SRR873442_filtered_2_8.fmt7</t>
-  </si>
-  <si>
     <t>PRJNA321261</t>
   </si>
   <si>
@@ -796,9 +772,6 @@
     <t>SRR3500418_mixcr.vdjca, SRR3500418_annotation.txt, SRR3500418.clns, SRR3500418_clones.txt</t>
   </si>
   <si>
-    <t>SRR3500418_a.txz, SRR3500418_b.txz</t>
-  </si>
-  <si>
     <t>PRJNA312319</t>
   </si>
   <si>
@@ -1060,9 +1033,6 @@
     <t>SRR3289698_mixcr.vdjca, SRR3289698_annotation.txt</t>
   </si>
   <si>
-    <t>SRR3289698_annotation.txt</t>
-  </si>
-  <si>
     <t>PRJNA356992</t>
   </si>
   <si>
@@ -1223,12 +1193,105 @@
   </si>
   <si>
     <t xml:space="preserve">IgG+, CD19+, sIgG+, negative depletion to CD3, CD14, CD16, IgM, IgA, IgD </t>
+  </si>
+  <si>
+    <t>IGHV</t>
+  </si>
+  <si>
+    <t>IGHC</t>
+  </si>
+  <si>
+    <t>454 Roche GS FLX</t>
+  </si>
+  <si>
+    <t>Adaptors and primers removed and igblast and imgt annotation of both quality filtered and unfiltered sequences</t>
+  </si>
+  <si>
+    <t>SRP018335</t>
+  </si>
+  <si>
+    <t>SAMN01908533</t>
+  </si>
+  <si>
+    <t>SRS388604</t>
+  </si>
+  <si>
+    <t>Zhu-PNAS</t>
+  </si>
+  <si>
+    <t>Heavy chain antibody repertoire sequencing from donor IAVI84 using 454 pyrosequencing platform</t>
+  </si>
+  <si>
+    <t>SRX220897</t>
+  </si>
+  <si>
+    <t>CCATCTCATCCCTGCGTGTC</t>
+  </si>
+  <si>
+    <t>CCTATCCCCTGTGTGCCTTG</t>
+  </si>
+  <si>
+    <t>TCCGACTCAGACAGGTGCCCACTCCCAGGTGCAG, TCCGACTCAGGCAGCCACAGGTGCCCACTCC, TCCGACTCAGCAGCAGCTACAGGCACCCACGC, TCCGACTCAGGGCAGCAGCTACAGGTGTCCAGTCC</t>
+  </si>
+  <si>
+    <t>GCAGTCTCAGGGGGAAGACCGATGGGCCCTTGGT, GCAGTCTCAGGGGAATTCTCACAGGAGACGA</t>
+  </si>
+  <si>
+    <t>BCR</t>
+  </si>
+  <si>
+    <t>IgHV1 Family</t>
+  </si>
+  <si>
+    <t>SRR654169</t>
+  </si>
+  <si>
+    <t>HIV-1 gp120 envelope glycoprotein</t>
+  </si>
+  <si>
+    <t>adapter, forward 5</t>
+  </si>
+  <si>
+    <t>filtered_SRR654169.fasta</t>
+  </si>
+  <si>
+    <t>filtered_SRR654169heavy_split1.txz</t>
+  </si>
+  <si>
+    <t>Each of the following rows contains the metdata that describes a repertoire sample and its processing.</t>
+  </si>
+  <si>
+    <t>The "Example Metadata" tab provides an example Metadata spreadsheet that could be used to load data. It consists of a set of rows that describe realistic repertoire samples from actual studies curated in the iReceptor Public Archiver repositories. The first row is a header row, and it is this row that defines the fields in the rest of the spreadsheet. If you are using this spreadsheet to load data into a repository using the iReceptor Data Loading software, these are the names of the fields that will be loaded into the repository. In general, we recommend that you use the AIRR Minimal Standard terms for these columns (these are the default columns provided).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bottom two rows should not be included as part of an iReceptor Metadata file. Rather these two rows are provided to give you more information on the content in the columns. The second to last row provides guidance on the expected "type" and/or content of the field. The bottom row contains an extended set of field names that the iReceptor project tracks in its metadata documentation but does not get added into the repository. You will note that there are some columns that do not have a field name in Row 1 but do have one in the bottom Row. Columns that do not have a field name in Row 1 are ignored by the data loader. If you want to store this data in the repository, simply assign a field name in Row 1 for that column. We recommend you prefix the column name with a unique prefix to differntiate that field from the AIRR columns. Special iReceptor columns are denoted with an ir_ prefix. These are columns that we track and store in the iReceptor repository. Many of them are required for the iReceptor Repositories to function correctly, so if you are using an iReceptor Repositroy please do not delete these columns. </t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Color Coding</t>
+  </si>
+  <si>
+    <t>Each of the rows that do not contain data are color coded to help understand the differenc columns.</t>
+  </si>
+  <si>
+    <t>The type row is colored in green to differntiate it from other rows.</t>
+  </si>
+  <si>
+    <t>Field names that are AIRR Community defined are colored in light green.</t>
+  </si>
+  <si>
+    <t>Field names that are iReceptor specific and saved in the iReceptor repositories are colored in light yellow.</t>
+  </si>
+  <si>
+    <t>Field names that the iReceptor Curators track but do not load into the iReceptor repositories are colored in Grey.</t>
   </si>
   <si>
     <r>
       <rPr>
         <vertAlign val="superscript"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1248,111 +1311,34 @@
     </r>
   </si>
   <si>
-    <t>IGHV</t>
-  </si>
-  <si>
-    <t>IGHC</t>
-  </si>
-  <si>
-    <t>454 Roche GS FLX</t>
-  </si>
-  <si>
-    <t>Adaptors and primers removed and igblast and imgt annotation of both quality filtered and unfiltered sequences</t>
-  </si>
-  <si>
-    <t>SRP018335</t>
-  </si>
-  <si>
-    <t>SAMN01908533</t>
-  </si>
-  <si>
-    <t>SRS388604</t>
-  </si>
-  <si>
-    <t>Zhu-PNAS</t>
-  </si>
-  <si>
-    <t>Heavy chain antibody repertoire sequencing from donor IAVI84 using 454 pyrosequencing platform</t>
-  </si>
-  <si>
-    <t>SRX220897</t>
-  </si>
-  <si>
-    <t>CCATCTCATCCCTGCGTGTC</t>
-  </si>
-  <si>
-    <t>CCTATCCCCTGTGTGCCTTG</t>
-  </si>
-  <si>
-    <t>TCCGACTCAGACAGGTGCCCACTCCCAGGTGCAG, TCCGACTCAGGCAGCCACAGGTGCCCACTCC, TCCGACTCAGCAGCAGCTACAGGCACCCACGC, TCCGACTCAGGGCAGCAGCTACAGGTGTCCAGTCC</t>
-  </si>
-  <si>
-    <t>GCAGTCTCAGGGGGAAGACCGATGGGCCCTTGGT, GCAGTCTCAGGGGAATTCTCACAGGAGACGA</t>
-  </si>
-  <si>
-    <t>BCR</t>
-  </si>
-  <si>
-    <t>IgHV1 Family</t>
-  </si>
-  <si>
-    <t>SRR654169</t>
-  </si>
-  <si>
-    <t>HIV-1 gp120 envelope glycoprotein</t>
-  </si>
-  <si>
-    <t>adapter, forward 5</t>
-  </si>
-  <si>
-    <t>filtered_SRR654169.fasta</t>
-  </si>
-  <si>
-    <t>filtered_SRR654169heavy_split1.txz</t>
-  </si>
-  <si>
-    <t>Each of the following rows contains the metdata that describes a repertoire sample and its processing.</t>
-  </si>
-  <si>
-    <t>The "Example Metadata" tab provides an example Metadata spreadsheet that could be used to load data. It consists of a set of rows that describe realistic repertoire samples from actual studies curated in the iReceptor Public Archiver repositories. The first row is a header row, and it is this row that defines the fields in the rest of the spreadsheet. If you are using this spreadsheet to load data into a repository using the iReceptor Data Loading software, these are the names of the fields that will be loaded into the repository. In general, we recommend that you use the AIRR Minimal Standard terms for these columns (these are the default columns provided).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The bottom two rows should not be included as part of an iReceptor Metadata file. Rather these two rows are provided to give you more information on the content in the columns. The second to last row provides guidance on the expected "type" and/or content of the field. The bottom row contains an extended set of field names that the iReceptor project tracks in its metadata documentation but does not get added into the repository. You will note that there are some columns that do not have a field name in Row 1 but do have one in the bottom Row. Columns that do not have a field name in Row 1 are ignored by the data loader. If you want to store this data in the repository, simply assign a field name in Row 1 for that column. We recommend you prefix the column name with a unique prefix to differntiate that field from the AIRR columns. Special iReceptor columns are denoted with an ir_ prefix. These are columns that we track and store in the iReceptor repository. Many of them are required for the iReceptor Repositories to function correctly, so if you are using an iReceptor Repositroy please do not delete these columns. </t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>Color Coding</t>
-  </si>
-  <si>
-    <t>Each of the rows that do not contain data are color coded to help understand the differenc columns.</t>
-  </si>
-  <si>
-    <t>The type row is colored in green to differntiate it from other rows.</t>
-  </si>
-  <si>
-    <t>Field names that are AIRR Community defined are colored in light green.</t>
-  </si>
-  <si>
-    <t>Field names that are iReceptor specific and saved in the iReceptor repositories are colored in light yellow.</t>
-  </si>
-  <si>
-    <t>Field names that the iReceptor Curators track but do not load into the iReceptor repositories are colored in Grey.</t>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">H.pylori </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and unknown</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1368,13 +1354,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -1383,20 +1362,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri (Body)"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1404,30 +1378,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Menlo"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1492,10 +1457,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1506,10 +1471,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1518,19 +1480,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1538,12 +1491,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1563,20 +1510,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1896,62 +1852,62 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="123.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="75">
-      <c r="A2" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="135">
-      <c r="A4" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="18.75">
-      <c r="A5" s="25" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="30" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="26" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="27" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="28" t="s">
-        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -1968,7 +1924,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
@@ -2080,289 +2036,289 @@
     <col min="110" max="110" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:110" ht="15" customHeight="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:110" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="Q1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="W1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="Y1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AA1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AB1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AC1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AE1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AF1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AG1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="18" t="s">
+      <c r="AH1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="AI1" s="18" t="s">
+      <c r="AI1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="18" t="s">
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="18" t="s">
+      <c r="AN1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="AO1" s="18" t="s">
+      <c r="AO1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="AP1" s="18" t="s">
+      <c r="AP1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="AQ1" s="18" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="18" t="s">
+      <c r="AR1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="18" t="s">
+      <c r="AS1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="AT1" s="18" t="s">
+      <c r="AT1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AU1" s="18" t="s">
+      <c r="AU1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="18" t="s">
+      <c r="AV1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="AW1" s="18" t="s">
+      <c r="AW1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="AX1" s="18" t="s">
+      <c r="AX1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AY1" s="18" t="s">
+      <c r="AY1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AZ1" s="18" t="s">
+      <c r="AZ1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="BA1" s="18" t="s">
+      <c r="BA1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="BB1" s="19" t="s">
+      <c r="BB1" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="BC1" s="18" t="s">
+      <c r="BC1" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="BD1" s="18" t="s">
+      <c r="BD1" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="BE1" s="18" t="s">
+      <c r="BE1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="BF1" s="18" t="s">
+      <c r="BF1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="BG1" s="18" t="s">
+      <c r="BG1" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="BH1" s="18" t="s">
+      <c r="BH1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="BI1" s="20" t="s">
+      <c r="BI1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="BJ1" s="18" t="s">
+      <c r="BJ1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="BK1" s="18" t="s">
+      <c r="BK1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="BL1" s="18" t="s">
+      <c r="BL1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="BM1" s="18" t="s">
+      <c r="BM1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="BN1" s="24"/>
-      <c r="BO1" s="18" t="s">
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="BP1" s="18" t="s">
+      <c r="BP1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="BQ1" s="18" t="s">
+      <c r="BQ1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="BR1" s="18" t="s">
+      <c r="BR1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="BS1" s="18" t="s">
+      <c r="BS1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="BT1" s="18" t="s">
+      <c r="BT1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="BU1" s="18" t="s">
+      <c r="BU1" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="BV1" s="18" t="s">
+      <c r="BV1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="BW1" s="18" t="s">
+      <c r="BW1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="BX1" s="18" t="s">
+      <c r="BX1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="BY1" s="18" t="s">
+      <c r="BY1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="BZ1" s="18" t="s">
+      <c r="BZ1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="CA1" s="17" t="s">
+      <c r="CA1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-      <c r="CD1" s="24"/>
-      <c r="CE1" s="17" t="s">
+      <c r="CB1" s="17"/>
+      <c r="CC1" s="17"/>
+      <c r="CD1" s="17"/>
+      <c r="CE1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="CF1" s="24"/>
-      <c r="CG1" s="24"/>
-      <c r="CH1" s="21" t="s">
+      <c r="CF1" s="17"/>
+      <c r="CG1" s="17"/>
+      <c r="CH1" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="CI1" s="24"/>
-      <c r="CJ1" s="24"/>
-      <c r="CK1" s="24"/>
-      <c r="CL1" s="24"/>
-      <c r="CM1" s="24"/>
-      <c r="CN1" s="24"/>
-      <c r="CO1" s="24"/>
-      <c r="CP1" s="24"/>
-      <c r="CQ1" s="24"/>
-      <c r="CR1" s="24"/>
-      <c r="CS1" s="24"/>
-      <c r="CT1" s="24"/>
-      <c r="CU1" s="24"/>
-      <c r="CV1" s="24"/>
-      <c r="CW1" s="24"/>
-      <c r="CX1" s="24"/>
-      <c r="CY1" s="24"/>
-      <c r="CZ1" s="17" t="s">
+      <c r="CI1" s="17"/>
+      <c r="CJ1" s="17"/>
+      <c r="CK1" s="17"/>
+      <c r="CL1" s="17"/>
+      <c r="CM1" s="17"/>
+      <c r="CN1" s="17"/>
+      <c r="CO1" s="17"/>
+      <c r="CP1" s="17"/>
+      <c r="CQ1" s="17"/>
+      <c r="CR1" s="17"/>
+      <c r="CS1" s="17"/>
+      <c r="CT1" s="17"/>
+      <c r="CU1" s="17"/>
+      <c r="CV1" s="17"/>
+      <c r="CW1" s="17"/>
+      <c r="CX1" s="17"/>
+      <c r="CY1" s="17"/>
+      <c r="CZ1" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="DA1" s="17" t="s">
+      <c r="DA1" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="DB1" s="17" t="s">
+      <c r="DB1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="DC1" s="17" t="s">
+      <c r="DC1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="DD1" s="17" t="s">
+      <c r="DD1" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="DE1" s="17" t="s">
+      <c r="DE1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="DF1" s="17" t="s">
+      <c r="DF1" s="11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:110" ht="15.75">
+    <row r="2" spans="1:110" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>31</v>
       </c>
@@ -2372,12 +2328,12 @@
       <c r="C2" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="23" t="s">
         <v>145</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>146</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -2407,10 +2363,10 @@
       <c r="P2" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="5">
         <v>75</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="5">
         <v>75</v>
       </c>
       <c r="S2" s="1" t="s">
@@ -2480,7 +2436,7 @@
       <c r="AU2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AV2" s="6">
+      <c r="AV2" s="5">
         <v>24201</v>
       </c>
       <c r="AW2" s="1" t="s">
@@ -2513,10 +2469,10 @@
         <v>174</v>
       </c>
       <c r="BL2" s="1"/>
-      <c r="BM2" s="6">
+      <c r="BM2" s="5">
         <v>341</v>
       </c>
-      <c r="BN2" s="6">
+      <c r="BN2" s="5">
         <v>341</v>
       </c>
       <c r="BO2" s="1" t="s">
@@ -2531,7 +2487,7 @@
         <v>176</v>
       </c>
       <c r="BV2" s="1"/>
-      <c r="BW2" s="6">
+      <c r="BW2" s="5">
         <v>25</v>
       </c>
       <c r="BX2" s="1"/>
@@ -2542,7 +2498,7 @@
       <c r="CA2" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CB2" s="6">
+      <c r="CB2" s="5">
         <v>2014</v>
       </c>
       <c r="CC2" s="1" t="s">
@@ -2603,30 +2559,32 @@
         <v>194</v>
       </c>
       <c r="CV2" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="CW2" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="CW2" s="1" t="s">
+      <c r="CX2" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="CX2" s="4" t="s">
+      <c r="CY2" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="CY2" s="4" t="s">
+      <c r="CZ2" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="CZ2" s="1" t="s">
+      <c r="DA2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="DA2" s="1" t="s">
+      <c r="DB2" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="DB2" s="1" t="s">
-        <v>201</v>
-      </c>
       <c r="DC2" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="DD2" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="DD2" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="DE2" s="1" t="s">
         <v>156</v>
       </c>
@@ -2634,42 +2592,42 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:110" ht="14.45" customHeight="1">
+    <row r="3" spans="1:110" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>605</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="M3" s="1" t="b">
         <v>0</v>
@@ -2678,15 +2636,15 @@
         <v>152</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q3" s="6">
+        <v>212</v>
+      </c>
+      <c r="Q3" s="5">
         <v>47</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>47</v>
       </c>
       <c r="S3" s="1" t="s">
@@ -2714,69 +2672,69 @@
         <v>157</v>
       </c>
       <c r="AA3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="AD3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AK3" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="AL3" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="AJ3" s="7" t="s">
+      <c r="AM3" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="AK3" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="AL3" s="7" t="s">
+      <c r="AN3" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>164</v>
       </c>
       <c r="AP3" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AS3" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="AU3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="AV3" s="6" t="s">
+      <c r="AV3" s="5" t="s">
         <v>156</v>
       </c>
       <c r="AW3" s="1" t="s">
@@ -2792,10 +2750,10 @@
         <v>156</v>
       </c>
       <c r="BA3" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="BB3" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BC3" s="1">
         <v>30</v>
@@ -2804,10 +2762,10 @@
         <v>156</v>
       </c>
       <c r="BE3" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BF3" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BG3" s="1" t="s">
         <v>156</v>
@@ -2816,10 +2774,10 @@
         <v>171</v>
       </c>
       <c r="BI3" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BJ3" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BK3" s="1" t="s">
         <v>174</v>
@@ -2827,17 +2785,17 @@
       <c r="BL3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BM3" s="6">
+      <c r="BM3" s="5">
         <v>875784</v>
       </c>
-      <c r="BN3" s="6">
+      <c r="BN3" s="5">
         <v>874105</v>
       </c>
       <c r="BO3" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="BP3" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="BQ3" s="1" t="s">
         <v>156</v>
@@ -2855,9 +2813,9 @@
         <v>176</v>
       </c>
       <c r="BV3" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="BW3" s="6">
+        <v>232</v>
+      </c>
+      <c r="BW3" s="5">
         <v>30</v>
       </c>
       <c r="BX3" s="1" t="s">
@@ -2872,47 +2830,47 @@
       <c r="CA3" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CB3" s="6">
+      <c r="CB3" s="5">
         <v>2016</v>
       </c>
       <c r="CC3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="CD3" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="CE3" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="CD3" s="8" t="s">
+      <c r="CF3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="CG3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CH3" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="CE3" s="1" t="s">
+      <c r="CI3" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="CF3" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="CG3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CH3" s="1" t="s">
+      <c r="CJ3" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="CI3" s="1" t="s">
+      <c r="CK3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CM3" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="CJ3" s="1" t="s">
+      <c r="CN3" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="CK3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CL3" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CM3" s="1" t="s">
+      <c r="CO3" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="CN3" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="CO3" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="CP3" s="1" t="s">
         <v>190</v>
@@ -2924,10 +2882,10 @@
         <v>156</v>
       </c>
       <c r="CS3" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="CT3" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CU3" s="1" t="s">
         <v>171</v>
@@ -2945,61 +2903,63 @@
         <v>156</v>
       </c>
       <c r="CZ3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="DA3" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="DB3" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="DA3" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="DB3" s="1" t="s">
-        <v>247</v>
-      </c>
       <c r="DC3" s="1" t="s">
         <v>156</v>
       </c>
       <c r="DD3" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="DE3" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="DE3" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="DF3" s="3">
         <v>615</v>
       </c>
     </row>
-    <row r="4" spans="1:110" ht="15.75">
-      <c r="A4" s="6">
+    <row r="4" spans="1:110" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>715</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="J4" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="K4" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="M4" s="1" t="b">
         <v>0</v>
@@ -3011,16 +2971,16 @@
         <v>153</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q4" s="10">
+        <v>257</v>
+      </c>
+      <c r="Q4" s="8">
         <v>4.3899999999999997</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="8">
         <v>4.3899999999999997</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>156</v>
@@ -3044,69 +3004,69 @@
         <v>157</v>
       </c>
       <c r="AA4" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AK4" s="24" t="s">
         <v>263</v>
       </c>
-      <c r="AG4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AL4" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AN4" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="AI4" s="1" t="s">
+      <c r="AO4" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AJ4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AK4" s="11" t="s">
+      <c r="AQ4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AS4" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="AL4" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="AM4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AN4" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="AO4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="AQ4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AR4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AS4" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="AU4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AV4" s="6">
+      <c r="AV4" s="5">
         <v>4856416</v>
       </c>
       <c r="AW4" s="1" t="s">
@@ -3122,34 +3082,34 @@
         <v>156</v>
       </c>
       <c r="BA4" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BB4" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BC4" s="1" t="s">
         <v>156</v>
       </c>
       <c r="BD4" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BE4" s="1" t="s">
         <v>170</v>
       </c>
       <c r="BF4" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BG4" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="BH4" s="1" t="s">
         <v>171</v>
       </c>
       <c r="BI4" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BJ4" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BK4" s="1" t="s">
         <v>174</v>
@@ -3157,107 +3117,107 @@
       <c r="BL4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BM4" s="6">
+      <c r="BM4" s="5">
         <v>4185236</v>
       </c>
-      <c r="BN4" s="6">
+      <c r="BN4" s="5">
         <v>4185236</v>
       </c>
       <c r="BO4" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="BP4" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="BQ4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BR4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BS4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BT4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BU4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="BV4" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="BP4" s="1" t="s">
+      <c r="BW4" s="5">
+        <v>30</v>
+      </c>
+      <c r="BX4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BY4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BZ4" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="BQ4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BR4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BS4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BT4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BU4" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="BV4" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="BW4" s="6">
-        <v>30</v>
-      </c>
-      <c r="BX4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BY4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="BZ4" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="CA4" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CB4" s="6">
+      <c r="CB4" s="5">
         <v>2017</v>
       </c>
       <c r="CC4" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="CD4" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="CE4" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="CG4" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="CD4" s="1" t="s">
+      <c r="CH4" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="CI4" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="CE4" s="1" t="s">
+      <c r="CJ4" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="CF4" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="CG4" s="1" t="s">
+      <c r="CK4" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="CH4" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="CI4" s="1" t="s">
+      <c r="CL4" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="CJ4" s="1" t="s">
+      <c r="CM4" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="CK4" s="1" t="s">
+      <c r="CN4" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="CL4" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="CM4" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="CN4" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="CO4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CP4" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CQ4" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="CR4" s="1" t="s">
         <v>156</v>
       </c>
       <c r="CS4" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="CT4" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CU4" s="1" t="s">
         <v>171</v>
@@ -3266,7 +3226,7 @@
         <v>156</v>
       </c>
       <c r="CW4" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="CX4" s="1" t="s">
         <v>156</v>
@@ -3275,13 +3235,13 @@
         <v>156</v>
       </c>
       <c r="CZ4" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="DA4" s="9" t="s">
-        <v>246</v>
+        <v>289</v>
+      </c>
+      <c r="DA4" s="23" t="s">
+        <v>244</v>
       </c>
       <c r="DB4" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="DC4" s="1" t="s">
         <v>156</v>
@@ -3289,47 +3249,49 @@
       <c r="DD4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="DE4" s="1"/>
-      <c r="DF4" s="6">
+      <c r="DE4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="DF4" s="5">
         <v>725</v>
       </c>
     </row>
-    <row r="5" spans="1:110" ht="15.6" customHeight="1">
+    <row r="5" spans="1:110" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>798</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="K5" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="M5" s="1" t="b">
         <v>0</v>
@@ -3341,92 +3303,92 @@
         <v>153</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>61</v>
+      </c>
+      <c r="R5" s="5">
+        <v>61</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="AA5" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="Q5" s="6">
-        <v>61</v>
-      </c>
-      <c r="R5" s="6">
-        <v>61</v>
-      </c>
-      <c r="S5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="AI5" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="AB5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AK5" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AP5" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="AN5" s="1" t="s">
+      <c r="AQ5" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="AR5" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="AO5" s="1" t="s">
+      <c r="AS5" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="AP5" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="AQ5" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="AR5" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="AS5" s="1" t="s">
-        <v>317</v>
       </c>
       <c r="AT5" s="1" t="s">
         <v>156</v>
@@ -3434,23 +3396,23 @@
       <c r="AU5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AV5" s="6">
+      <c r="AV5" s="5">
         <v>2731777</v>
       </c>
       <c r="AW5" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AX5" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="AY5" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AZ5" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="BA5" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="BB5" s="1" t="s">
         <v>169</v>
@@ -3465,7 +3427,7 @@
         <v>170</v>
       </c>
       <c r="BF5" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="BG5" s="1" t="s">
         <v>156</v>
@@ -3474,10 +3436,10 @@
         <v>171</v>
       </c>
       <c r="BI5" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BJ5" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BK5" s="1" t="s">
         <v>174</v>
@@ -3485,20 +3447,20 @@
       <c r="BL5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BM5" s="6">
+      <c r="BM5" s="5">
         <v>1787205</v>
       </c>
-      <c r="BN5" s="6">
+      <c r="BN5" s="5">
         <v>992813</v>
       </c>
       <c r="BO5" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="BP5" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="BQ5" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="BR5" s="1"/>
       <c r="BS5" s="1" t="s">
@@ -3508,12 +3470,12 @@
         <v>156</v>
       </c>
       <c r="BU5" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="BV5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BW5" s="6">
+      <c r="BW5" s="5">
         <v>30</v>
       </c>
       <c r="BX5" s="1" t="s">
@@ -3523,25 +3485,25 @@
         <v>156</v>
       </c>
       <c r="BZ5" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="CA5" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CB5" s="6">
+      <c r="CB5" s="5">
         <v>2016</v>
       </c>
       <c r="CC5" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="CD5" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="CE5" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="CF5" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="CD5" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="CE5" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="CF5" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="CG5" s="1" t="s">
         <v>156</v>
@@ -3550,37 +3512,37 @@
         <v>184</v>
       </c>
       <c r="CI5" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="CJ5" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="CK5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CL5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CM5" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="CN5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CO5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="CP5" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="CQ5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CR5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CS5" s="1" t="s">
         <v>329</v>
-      </c>
-      <c r="CK5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CL5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CM5" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="CN5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CO5" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="CP5" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="CQ5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CR5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CS5" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="CT5" s="1" t="s">
         <v>193</v>
@@ -3592,7 +3554,7 @@
         <v>156</v>
       </c>
       <c r="CW5" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="CX5" s="1" t="s">
         <v>156</v>
@@ -3601,59 +3563,63 @@
         <v>156</v>
       </c>
       <c r="CZ5" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="DA5" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="DB5" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="DC5" s="1"/>
-      <c r="DD5" s="1"/>
+        <v>332</v>
+      </c>
+      <c r="DC5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD5" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="DE5" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="DF5" s="6">
+        <v>332</v>
+      </c>
+      <c r="DF5" s="5">
         <v>808</v>
       </c>
     </row>
-    <row r="6" spans="1:110" ht="16.899999999999999" customHeight="1">
+    <row r="6" spans="1:110" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>861</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="M6" s="1" t="b">
         <v>0</v>
@@ -3662,110 +3628,110 @@
         <v>152</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="P6" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>65</v>
+      </c>
+      <c r="R6" s="5">
+        <v>65</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH6" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="Q6" s="6">
-        <v>65</v>
-      </c>
-      <c r="R6" s="6">
-        <v>65</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="Z6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AJ6" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="AB6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AK6" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AM6" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="AD6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH6" s="1" t="s">
+      <c r="AN6" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AO6" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="AI6" s="1" t="s">
+      <c r="AP6" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
         <v>352</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="AP6" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="AQ6" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="AU6" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AV6" s="6">
+      <c r="AV6" s="5">
         <v>5611906</v>
       </c>
       <c r="AW6" s="1" t="s">
         <v>156</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="AY6" s="1" t="s">
         <v>156</v>
@@ -3774,7 +3740,7 @@
         <v>156</v>
       </c>
       <c r="BA6" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="BB6" s="1" t="s">
         <v>169</v>
@@ -3783,25 +3749,25 @@
         <v>156</v>
       </c>
       <c r="BD6" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="BE6" s="1" t="s">
         <v>170</v>
       </c>
       <c r="BF6" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="BG6" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="BH6" s="1" t="s">
         <v>171</v>
       </c>
       <c r="BI6" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="BJ6" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="BK6" s="1" t="s">
         <v>174</v>
@@ -3809,17 +3775,17 @@
       <c r="BL6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="BM6" s="6">
+      <c r="BM6" s="5">
         <v>2187622</v>
       </c>
-      <c r="BN6" s="6">
+      <c r="BN6" s="5">
         <v>2109470</v>
       </c>
       <c r="BO6" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="BP6" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="BQ6" s="1" t="s">
         <v>156</v>
@@ -3834,12 +3800,12 @@
         <v>156</v>
       </c>
       <c r="BU6" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="BV6" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="BW6" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="BW6" s="5" t="s">
         <v>156</v>
       </c>
       <c r="BX6" s="1" t="s">
@@ -3849,67 +3815,67 @@
         <v>156</v>
       </c>
       <c r="BZ6" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="CA6" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CB6" s="6">
+      <c r="CB6" s="5">
         <v>2017</v>
       </c>
       <c r="CC6" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="CD6" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="CE6" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="CF6" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="CG6" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="CH6" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="CI6" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="CJ6" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="CD6" s="1" t="s">
+      <c r="CK6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CL6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CM6" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CE6" s="1" t="s">
+      <c r="CN6" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="CF6" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="CG6" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="CH6" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="CI6" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="CJ6" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="CK6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CL6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CM6" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="CN6" s="1" t="s">
-        <v>372</v>
-      </c>
       <c r="CO6" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CP6" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CQ6" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="CR6" s="1" t="s">
         <v>156</v>
       </c>
       <c r="CS6" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="CT6" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CU6" s="1" t="s">
         <v>171</v>
@@ -3927,53 +3893,59 @@
         <v>156</v>
       </c>
       <c r="CZ6" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="DA6" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="DB6" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="DC6" s="1"/>
-      <c r="DD6" s="1"/>
-      <c r="DE6" s="1"/>
-      <c r="DF6" s="6">
+        <v>371</v>
+      </c>
+      <c r="DC6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DE6" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="DF6" s="5">
         <v>896</v>
       </c>
     </row>
-    <row r="7" spans="1:110" ht="15" customHeight="1">
+    <row r="7" spans="1:110" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>378</v>
+        <v>373</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>374</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="L7" s="9" t="s">
         <v>380</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>384</v>
       </c>
       <c r="M7" s="1" t="b">
         <v>0</v>
@@ -3985,12 +3957,12 @@
         <v>156</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q7" s="6">
+        <v>381</v>
+      </c>
+      <c r="Q7" s="5">
         <v>18</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="5">
         <v>999</v>
       </c>
       <c r="S7" s="1" t="s">
@@ -4016,10 +3988,10 @@
         <v>157</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
@@ -4028,20 +4000,20 @@
       <c r="AG7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AH7" s="13" t="s">
-        <v>388</v>
+      <c r="AH7" s="9" t="s">
+        <v>384</v>
       </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="AO7" s="1" t="s">
         <v>164</v>
@@ -4052,26 +4024,26 @@
       <c r="AQ7" s="1"/>
       <c r="AR7" s="1"/>
       <c r="AS7" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AT7" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="AU7" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="AV7" s="6">
+      <c r="AV7" s="5">
         <v>279503</v>
       </c>
       <c r="AW7" s="1" t="s">
-        <v>391</v>
+        <v>418</v>
       </c>
       <c r="AX7" s="1"/>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
       <c r="BB7" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="BC7" s="1"/>
       <c r="BD7" s="1"/>
@@ -4084,23 +4056,23 @@
         <v>171</v>
       </c>
       <c r="BI7" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="BJ7" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="BK7" s="1" t="s">
         <v>174</v>
       </c>
       <c r="BL7" s="1"/>
-      <c r="BM7" s="23">
+      <c r="BM7" s="25">
         <v>253683</v>
       </c>
-      <c r="BN7" s="23">
+      <c r="BN7" s="25">
         <v>253683</v>
       </c>
       <c r="BO7" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
@@ -4111,847 +4083,851 @@
         <v>176</v>
       </c>
       <c r="BV7" s="1"/>
-      <c r="BW7" s="6">
+      <c r="BW7" s="5">
         <v>30</v>
       </c>
       <c r="BX7" s="1"/>
       <c r="BY7" s="1"/>
       <c r="BZ7" s="1" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="CA7" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="CB7" s="6">
+      <c r="CB7" s="5">
         <v>2013</v>
       </c>
       <c r="CC7" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="CD7" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="CE7" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="CF7" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="CG7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CH7" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="CI7" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="CJ7" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="CD7" s="1" t="s">
+      <c r="CK7" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="CE7" s="1" t="s">
+      <c r="CL7" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="CF7" s="1" t="s">
+      <c r="CM7" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="CG7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CH7" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="CI7" s="1" t="s">
+      <c r="CN7" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="CJ7" s="1" t="s">
+      <c r="CO7" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="CK7" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="CL7" s="4" t="s">
-        <v>403</v>
-      </c>
-      <c r="CM7" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="CN7" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="CO7" s="1" t="s">
-        <v>406</v>
       </c>
       <c r="CP7" s="1" t="s">
         <v>190</v>
       </c>
       <c r="CQ7" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="CR7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CS7" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="CT7" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="CU7" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="CV7" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="CW7" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="CX7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CY7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="CZ7" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="DA7" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="DB7" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="CR7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CS7" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="CT7" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="CU7" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="CV7" s="15" t="s">
-        <v>409</v>
-      </c>
-      <c r="CW7" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="CX7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CY7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="CZ7" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="DA7" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="DB7" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="DC7" s="1"/>
-      <c r="DD7" s="1"/>
+      <c r="DC7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD7" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="DE7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="DF7" s="6">
+      <c r="DF7" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:110" s="16" customFormat="1">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:110" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="29" t="s">
+      <c r="E8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="L8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="M8" s="29" t="s">
+      <c r="L8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="M8" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="O8" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="P8" s="29" t="s">
+      <c r="P8" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="Q8" s="29" t="s">
+      <c r="Q8" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="R8" s="29" t="s">
+      <c r="R8" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="S8" s="29" t="s">
+      <c r="S8" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="T8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="U8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="V8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="W8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="X8" s="29" t="s">
+      <c r="T8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="U8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="V8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="W8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="X8" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="Y8" s="29" t="s">
+      <c r="Y8" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="Z8" s="29" t="s">
+      <c r="Z8" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AA8" s="29" t="s">
+      <c r="AA8" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="AB8" s="29" t="s">
+      <c r="AB8" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="AC8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AE8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI8" s="29" t="s">
+      <c r="AC8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI8" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="AJ8" s="29" t="s">
+      <c r="AJ8" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="AK8" s="29"/>
-      <c r="AL8" s="29"/>
-      <c r="AM8" s="29" t="s">
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
+      <c r="AM8" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="AN8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AO8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AP8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AQ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AR8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AS8" s="29" t="s">
+      <c r="AN8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AO8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AP8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AQ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AR8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AS8" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="AT8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU8" s="29" t="s">
+      <c r="AT8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU8" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AV8" s="29" t="s">
+      <c r="AV8" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="AW8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AX8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AY8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="AZ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BA8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BB8" s="29" t="s">
+      <c r="AW8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AX8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="AZ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BA8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB8" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="BC8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BD8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BE8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BF8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BG8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BH8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BI8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BJ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BK8" s="29" t="s">
+      <c r="BC8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BE8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BH8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BI8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BJ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BK8" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="BL8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM8" s="29" t="s">
+      <c r="BL8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BM8" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="BN8" s="29" t="s">
+      <c r="BN8" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="BO8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BP8" s="29" t="s">
+      <c r="BO8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BP8" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="BQ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BR8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BS8" s="29" t="s">
+      <c r="BQ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BR8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BS8" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="BT8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BU8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BV8" s="29" t="s">
+      <c r="BT8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BU8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BV8" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="BW8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BX8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BY8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="BZ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CA8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CB8" s="29" t="s">
+      <c r="BW8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BX8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BY8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="BZ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CA8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CB8" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="CC8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CD8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CE8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CF8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CG8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CH8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CI8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CJ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CK8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CL8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CM8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CN8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CO8" s="29" t="s">
+      <c r="CC8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CD8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CE8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CF8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CH8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CI8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CJ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CK8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CL8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CM8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CN8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CO8" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="CP8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CQ8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CR8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CS8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CT8" s="29" t="s">
+      <c r="CP8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CQ8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CR8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CS8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CT8" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="CU8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CV8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CW8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CX8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CY8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="CZ8" s="29" t="s">
+      <c r="CU8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CV8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CW8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CX8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CY8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="CZ8" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="DA8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="DB8" s="29" t="s">
+      <c r="DA8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="DB8" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="DC8" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="DD8" s="29" t="s">
+      <c r="DC8" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="DD8" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="DE8" s="29" t="s">
+      <c r="DE8" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="DF8" s="29" t="s">
+      <c r="DF8" s="26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:110" s="22" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="17" t="str">
+    <row r="9" spans="1:110" s="16" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="str">
         <f>A1</f>
         <v>ir_record_number</v>
       </c>
-      <c r="B9" s="18" t="str">
+      <c r="B9" s="12" t="str">
         <f t="shared" ref="B9:AJ9" si="0">B1</f>
         <v>study_id</v>
       </c>
-      <c r="C9" s="18" t="str">
+      <c r="C9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>study_title</v>
       </c>
-      <c r="D9" s="18" t="str">
+      <c r="D9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>study_description</v>
       </c>
-      <c r="E9" s="18" t="str">
+      <c r="E9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>inclusion_exclusion_criteria</v>
       </c>
-      <c r="F9" s="18" t="str">
+      <c r="F9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>grants</v>
       </c>
-      <c r="G9" s="18" t="str">
+      <c r="G9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>collected_by</v>
       </c>
-      <c r="H9" s="18" t="str">
+      <c r="H9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>lab_name</v>
       </c>
-      <c r="I9" s="18" t="str">
+      <c r="I9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>lab_address</v>
       </c>
-      <c r="J9" s="18" t="str">
+      <c r="J9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>submitted_by</v>
       </c>
-      <c r="K9" s="18" t="str">
+      <c r="K9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>pub_ids</v>
       </c>
-      <c r="L9" s="18" t="str">
+      <c r="L9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>subject_id</v>
       </c>
-      <c r="M9" s="18" t="str">
+      <c r="M9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>synthetic</v>
       </c>
-      <c r="N9" s="18" t="str">
+      <c r="N9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>organism</v>
       </c>
-      <c r="O9" s="18" t="str">
+      <c r="O9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>sex</v>
       </c>
-      <c r="P9" s="18" t="str">
+      <c r="P9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>age</v>
       </c>
-      <c r="Q9" s="17" t="str">
+      <c r="Q9" s="11" t="str">
         <f t="shared" si="0"/>
         <v>ir_min_age</v>
       </c>
-      <c r="R9" s="17" t="str">
+      <c r="R9" s="11" t="str">
         <f t="shared" si="0"/>
         <v>ir_max_age</v>
       </c>
-      <c r="S9" s="18" t="str">
+      <c r="S9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>age_event</v>
       </c>
-      <c r="T9" s="18" t="str">
+      <c r="T9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>ancestry_population</v>
       </c>
-      <c r="U9" s="18" t="str">
+      <c r="U9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>ethnicity</v>
       </c>
-      <c r="V9" s="18" t="str">
+      <c r="V9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>race</v>
       </c>
-      <c r="W9" s="18" t="str">
+      <c r="W9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>strain_name</v>
       </c>
-      <c r="X9" s="18" t="str">
+      <c r="X9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>linked_subjects</v>
       </c>
-      <c r="Y9" s="18" t="str">
+      <c r="Y9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>link_type</v>
       </c>
-      <c r="Z9" s="18" t="str">
+      <c r="Z9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>study_group_description</v>
       </c>
-      <c r="AA9" s="18" t="str">
+      <c r="AA9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>disease_diagnosis</v>
       </c>
-      <c r="AB9" s="18" t="str">
+      <c r="AB9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>disease_length</v>
       </c>
-      <c r="AC9" s="18" t="str">
+      <c r="AC9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>disease_stage</v>
       </c>
-      <c r="AD9" s="18" t="str">
+      <c r="AD9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>prior_therapies</v>
       </c>
-      <c r="AE9" s="18" t="str">
+      <c r="AE9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>immunogen</v>
       </c>
-      <c r="AF9" s="18" t="str">
+      <c r="AF9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>intervention</v>
       </c>
-      <c r="AG9" s="18" t="str">
+      <c r="AG9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>medical_history</v>
       </c>
-      <c r="AH9" s="18" t="str">
+      <c r="AH9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>sample_id</v>
       </c>
-      <c r="AI9" s="18" t="str">
+      <c r="AI9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>sample_type</v>
       </c>
-      <c r="AJ9" s="18" t="str">
+      <c r="AJ9" s="12" t="str">
         <f t="shared" si="0"/>
         <v>tissue</v>
       </c>
-      <c r="AK9" s="24" t="s">
+      <c r="AK9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="AL9" s="24" t="s">
+      <c r="AL9" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AM9" s="18" t="str">
+      <c r="AM9" s="12" t="str">
         <f t="shared" ref="AM9:CA9" si="1">AM1</f>
         <v>anatomic_site</v>
       </c>
-      <c r="AN9" s="18" t="str">
+      <c r="AN9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>disease_state_sample</v>
       </c>
-      <c r="AO9" s="18" t="str">
+      <c r="AO9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>collection_time_point_relative</v>
       </c>
-      <c r="AP9" s="18" t="str">
+      <c r="AP9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>collection_time_point_reference</v>
       </c>
-      <c r="AQ9" s="18" t="str">
+      <c r="AQ9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>biomaterial_provider</v>
       </c>
-      <c r="AR9" s="18" t="str">
+      <c r="AR9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>tissue_processing</v>
       </c>
-      <c r="AS9" s="18" t="str">
+      <c r="AS9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_subset</v>
       </c>
-      <c r="AT9" s="18" t="str">
+      <c r="AT9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_phenotype</v>
       </c>
-      <c r="AU9" s="18" t="str">
+      <c r="AU9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>single_cell</v>
       </c>
-      <c r="AV9" s="18" t="str">
+      <c r="AV9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_number</v>
       </c>
-      <c r="AW9" s="18" t="str">
+      <c r="AW9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cells_per_reaction</v>
       </c>
-      <c r="AX9" s="18" t="str">
+      <c r="AX9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_storage</v>
       </c>
-      <c r="AY9" s="18" t="str">
+      <c r="AY9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_quality</v>
       </c>
-      <c r="AZ9" s="18" t="str">
+      <c r="AZ9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_isolation</v>
       </c>
-      <c r="BA9" s="18" t="str">
+      <c r="BA9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>cell_processing_protocol</v>
       </c>
-      <c r="BB9" s="18" t="str">
+      <c r="BB9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>template_class</v>
       </c>
-      <c r="BC9" s="18" t="str">
+      <c r="BC9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>template_quality</v>
       </c>
-      <c r="BD9" s="18" t="str">
+      <c r="BD9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>template_amount</v>
       </c>
-      <c r="BE9" s="18" t="str">
+      <c r="BE9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>library_generation_method</v>
       </c>
-      <c r="BF9" s="18" t="str">
+      <c r="BF9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>library_generation_protocol</v>
       </c>
-      <c r="BG9" s="18" t="str">
+      <c r="BG9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>library_generation_kit_version</v>
       </c>
-      <c r="BH9" s="18" t="str">
+      <c r="BH9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>pcr_target_locus</v>
       </c>
-      <c r="BI9" s="18" t="str">
+      <c r="BI9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>forward_pcr_primer_target_location</v>
       </c>
-      <c r="BJ9" s="18" t="str">
+      <c r="BJ9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>reverse_pcr_primer_target_location</v>
       </c>
-      <c r="BK9" s="18" t="str">
+      <c r="BK9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>complete_sequences</v>
       </c>
-      <c r="BL9" s="18" t="str">
+      <c r="BL9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>physical_linkage</v>
       </c>
-      <c r="BM9" s="18" t="str">
+      <c r="BM9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>total_reads_passing_qc_filter</v>
       </c>
-      <c r="BN9" s="24" t="s">
+      <c r="BN9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="BO9" s="18" t="str">
+      <c r="BO9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>sequencing_platform</v>
       </c>
-      <c r="BP9" s="18" t="str">
+      <c r="BP9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>read_length</v>
       </c>
-      <c r="BQ9" s="18" t="str">
+      <c r="BQ9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>sequencing_facility</v>
       </c>
-      <c r="BR9" s="18" t="str">
+      <c r="BR9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>sequencing_run_id</v>
       </c>
-      <c r="BS9" s="18" t="str">
+      <c r="BS9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>sequencing_run_date</v>
       </c>
-      <c r="BT9" s="18" t="str">
+      <c r="BT9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>sequencing_kit</v>
       </c>
-      <c r="BU9" s="18" t="str">
+      <c r="BU9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>software_versions</v>
       </c>
-      <c r="BV9" s="18" t="str">
+      <c r="BV9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>paired_read_assembly</v>
       </c>
-      <c r="BW9" s="18" t="str">
+      <c r="BW9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>quality_thresholds</v>
       </c>
-      <c r="BX9" s="18" t="str">
+      <c r="BX9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>primer_match_cutoffs</v>
       </c>
-      <c r="BY9" s="18" t="str">
+      <c r="BY9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>collapsing_method</v>
       </c>
-      <c r="BZ9" s="18" t="str">
+      <c r="BZ9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>data_processing_protocols</v>
       </c>
-      <c r="CA9" s="17" t="str">
+      <c r="CA9" s="11" t="str">
         <f t="shared" si="1"/>
         <v>ir_germline_database</v>
       </c>
-      <c r="CB9" s="24" t="s">
+      <c r="CB9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="CC9" s="24" t="s">
+      <c r="CC9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="CD9" s="24" t="s">
+      <c r="CD9" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="CE9" s="17" t="s">
+      <c r="CE9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="CF9" s="24" t="s">
+      <c r="CF9" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="CG9" s="24" t="s">
+      <c r="CG9" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="CH9" s="17" t="str">
+      <c r="CH9" s="11" t="str">
         <f>CH1</f>
         <v>ir_library_source</v>
       </c>
-      <c r="CI9" s="24" t="s">
+      <c r="CI9" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="CJ9" s="24" t="s">
+      <c r="CJ9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="CK9" s="24" t="s">
+      <c r="CK9" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="CL9" s="24" t="s">
+      <c r="CL9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="CM9" s="24" t="s">
+      <c r="CM9" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="CN9" s="24" t="s">
+      <c r="CN9" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="CO9" s="24" t="s">
+      <c r="CO9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="CP9" s="24" t="s">
+      <c r="CP9" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="CQ9" s="24" t="s">
+      <c r="CQ9" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="CR9" s="24" t="s">
+      <c r="CR9" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="CS9" s="24" t="s">
+      <c r="CS9" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="CT9" s="24" t="s">
+      <c r="CT9" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="CU9" s="24" t="s">
+      <c r="CU9" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="CV9" s="24" t="s">
+      <c r="CV9" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="CW9" s="24" t="s">
+      <c r="CW9" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="CX9" s="24" t="s">
+      <c r="CX9" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="CY9" s="24" t="s">
+      <c r="CY9" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="CZ9" s="17" t="str">
+      <c r="CZ9" s="11" t="str">
         <f>CZ1</f>
         <v>ir_fasta_file_name</v>
       </c>
-      <c r="DA9" s="17" t="str">
+      <c r="DA9" s="11" t="str">
         <f t="shared" ref="DA9:DF9" si="2">DA1</f>
         <v>ir_rearrangement_tool</v>
       </c>
-      <c r="DB9" s="17" t="str">
+      <c r="DB9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>ir_rearrangement_file_name</v>
       </c>
-      <c r="DC9" s="17" t="str">
+      <c r="DC9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>ir_igblast_file_name</v>
       </c>
-      <c r="DD9" s="17" t="str">
+      <c r="DD9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>ir_imgt_file_name</v>
       </c>
-      <c r="DE9" s="17" t="str">
+      <c r="DE9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>ir_mixcr_file_name</v>
       </c>
-      <c r="DF9" s="17" t="str">
+      <c r="DF9" s="11" t="str">
         <f t="shared" si="2"/>
         <v>ir_rearrangement_number</v>
       </c>

</xml_diff>

<commit_message>
Added color coding for mandatory AIRR fields.
</commit_message>
<xml_diff>
--- a/metadata/iReceptor_example_metadata_outline.xlsx
+++ b/metadata/iReceptor_example_metadata_outline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcorrie\Documents\Source\dataloading-curation\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5958FF7-3BED-4C32-932A-FAD86AAD3E8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6324F0A8-0F0E-4897-B0AB-176B3B5610A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="885" windowWidth="26220" windowHeight="11400" activeTab="1" xr2:uid="{34AD7A3A-B4E1-4AE0-8A8A-2D7A7A71B3DB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{34AD7A3A-B4E1-4AE0-8A8A-2D7A7A71B3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="2" r:id="rId1"/>
@@ -663,9 +663,6 @@
     <t>Each of the rows that do not contain data are color coded to help understand the differenc columns.</t>
   </si>
   <si>
-    <t>Field names that are AIRR Community defined are colored in light green.</t>
-  </si>
-  <si>
     <t>repertoire_id</t>
   </si>
   <si>
@@ -1258,6 +1255,9 @@
   </si>
   <si>
     <t>Field names that are custom (e.g. user defined) such as iReceptor fields are colored in yellow</t>
+  </si>
+  <si>
+    <t>Field names that are AIRR Community defined are colored in light green. Where a column is all green, that column is an AIRR Mandatory field and must be provided.</t>
   </si>
 </sst>
 </file>
@@ -1411,7 +1411,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1469,6 +1468,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -1804,7 +1806,7 @@
     </row>
     <row r="2" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -1814,7 +1816,7 @@
     </row>
     <row r="4" spans="1:1" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -1828,18 +1830,18 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>405</v>
+      <c r="A7" s="11" t="s">
+        <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>209</v>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>407</v>
+      <c r="A9" s="31" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -1853,7 +1855,7 @@
   <dimension ref="A1:CV9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="BT22" sqref="BT22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,305 +1956,305 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:100" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="R1" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="V1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="Y1" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Z1" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AA1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="AA1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AK1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT1" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AK1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AQ1" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AS1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AU1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="BA1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB1" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="AU1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="AV1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="AW1" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="AX1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY1" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AZ1" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="BA1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="BB1" s="16" t="s">
+      <c r="BC1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="BD1" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="BC1" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="BD1" s="14" t="s">
+      <c r="BE1" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="BE1" s="14" t="s">
+      <c r="BF1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="BH1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="BK1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="BL1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="BM1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="BP1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="BR1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="BS1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="BU1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="BW1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="BX1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="BY1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="BZ1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="CA1" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="BF1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="BG1" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="BH1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="BI1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="BJ1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="BK1" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="BL1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="BM1" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="BN1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="BO1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="BP1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ1" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="BR1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="BS1" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="BT1" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="BU1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="BW1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="BX1" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="BY1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="BZ1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="CA1" s="14" t="s">
+      <c r="CB1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="CC1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="CD1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="CE1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="CF1" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="CB1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="CC1" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="CD1" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="CE1" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="CF1" s="14" t="s">
+      <c r="CG1" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="CG1" s="14" t="s">
+      <c r="CH1" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="CH1" s="14" t="s">
+      <c r="CI1" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="CI1" s="14" t="s">
+      <c r="CJ1" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="CJ1" s="14" t="s">
+      <c r="CK1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="CL1" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="CK1" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="CL1" s="14" t="s">
+      <c r="CM1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="CN1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="CO1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="CP1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="CQ1" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="CM1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="CN1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="CO1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="CP1" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="CQ1" s="14" t="s">
+      <c r="CR1" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="CR1" s="14" t="s">
+      <c r="CS1" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="CS1" s="14" t="s">
+      <c r="CT1" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="CT1" s="14" t="s">
+      <c r="CU1" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="CU1" s="14" t="s">
+      <c r="CV1" s="13" t="s">
         <v>238</v>
-      </c>
-      <c r="CV1" s="14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:100" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -2271,12 +2273,12 @@
         <v>190</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>191</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -2292,7 +2294,7 @@
         <v>195</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q2" s="1" t="str">
         <f>IF(LEFT(BS2,2)="IG","contains_ig",IF(LEFT(BS2,2)="TR", "contains_tcr",""))</f>
@@ -2301,17 +2303,17 @@
       <c r="R2" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="S2" s="1" t="b">
+      <c r="S2" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="W2" s="8">
         <v>18</v>
@@ -2321,7 +2323,7 @@
         <v>49</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AA2" s="1" t="s">
         <v>80</v>
@@ -2330,10 +2332,10 @@
         <v>81</v>
       </c>
       <c r="AI2" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="AJ2" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="AJ2" s="20" t="s">
-        <v>247</v>
       </c>
       <c r="AK2" s="1" t="s">
         <v>197</v>
@@ -2342,10 +2344,10 @@
         <v>198</v>
       </c>
       <c r="AS2" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="AV2" s="1" t="s">
         <v>199</v>
@@ -2356,8 +2358,8 @@
       <c r="AX2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BB2" s="20" t="s">
-        <v>250</v>
+      <c r="BB2" s="19" t="s">
+        <v>249</v>
       </c>
       <c r="BD2" s="1" t="s">
         <v>79</v>
@@ -2372,20 +2374,20 @@
       <c r="BG2" s="5">
         <v>279503</v>
       </c>
-      <c r="BH2" s="21">
+      <c r="BH2" s="20">
         <v>15000000</v>
       </c>
       <c r="BI2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BM2" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BP2" s="13" t="s">
         <v>89</v>
       </c>
       <c r="BS2" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BT2" s="1" t="s">
         <v>200</v>
@@ -2393,28 +2395,28 @@
       <c r="BU2" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BV2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW2" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="BW2" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="BX2" s="22">
+      <c r="BX2" s="21">
         <v>253683</v>
       </c>
       <c r="BY2" s="1" t="s">
         <v>202</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CG2" s="1" t="s">
         <v>204</v>
       </c>
       <c r="CK2" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="CM2" s="20">
+        <v>254</v>
+      </c>
+      <c r="CM2" s="19">
         <v>30</v>
       </c>
       <c r="CP2" s="1" t="s">
@@ -2428,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="CS2" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="CT2" s="5">
         <f t="shared" ref="CT2:CT7" si="1">A2</f>
@@ -2457,12 +2459,12 @@
         <v>72</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>73</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -2478,7 +2480,7 @@
         <v>77</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q3" s="1" t="str">
         <f t="shared" ref="Q3:Q7" si="2">IF(LEFT(BS3,2)="IG","contains_ig",IF(LEFT(BS3,2)="TR", "contains_tcr",""))</f>
@@ -2487,17 +2489,17 @@
       <c r="R3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S3" s="1" t="b">
+      <c r="S3" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>243</v>
+      <c r="U3" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W3" s="8">
         <v>75</v>
@@ -2509,7 +2511,7 @@
         <v>49</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>80</v>
@@ -2518,10 +2520,10 @@
         <v>81</v>
       </c>
       <c r="AI3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AJ3" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="AJ3" s="20" t="s">
-        <v>262</v>
       </c>
       <c r="AQ3" s="1" t="s">
         <v>82</v>
@@ -2530,10 +2532,10 @@
         <v>83</v>
       </c>
       <c r="AS3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AT3" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="AV3" s="1" t="s">
         <v>84</v>
@@ -2545,10 +2547,10 @@
         <v>86</v>
       </c>
       <c r="BA3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="BB3" s="19" t="s">
         <v>265</v>
-      </c>
-      <c r="BB3" s="20" t="s">
-        <v>266</v>
       </c>
       <c r="BC3" s="1" t="s">
         <v>87</v>
@@ -2566,21 +2568,21 @@
       <c r="BG3" s="5">
         <v>24201</v>
       </c>
-      <c r="BH3" s="21">
+      <c r="BH3" s="20">
         <f t="shared" ref="BH3" si="3">10^9</f>
         <v>1000000000</v>
       </c>
       <c r="BI3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="BM3" s="1" t="s">
+      <c r="BM3" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="BP3" s="1" t="s">
+      <c r="BP3" s="13" t="s">
         <v>89</v>
       </c>
       <c r="BS3" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BT3" s="1" t="s">
         <v>90</v>
@@ -2588,11 +2590,11 @@
       <c r="BU3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BV3" s="1" t="s">
+      <c r="BV3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW3" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="BW3" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="BX3" s="5">
         <v>341</v>
@@ -2601,15 +2603,15 @@
         <v>92</v>
       </c>
       <c r="CF3" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CG3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="CK3" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="CM3" s="20">
+        <v>254</v>
+      </c>
+      <c r="CM3" s="19">
         <v>25</v>
       </c>
       <c r="CP3" s="1" t="s">
@@ -2652,10 +2654,10 @@
         <v>98</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>73</v>
@@ -2679,7 +2681,7 @@
         <v>104</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q4" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2688,17 +2690,17 @@
       <c r="R4" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="S4" s="1" t="b">
+      <c r="S4" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>243</v>
+      <c r="U4" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W4" s="8">
         <v>47</v>
@@ -2710,7 +2712,7 @@
         <v>49</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>80</v>
@@ -2718,11 +2720,11 @@
       <c r="AH4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AI4" s="24" t="s">
+      <c r="AI4" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="AJ4" s="24" t="s">
         <v>269</v>
-      </c>
-      <c r="AJ4" s="25" t="s">
-        <v>270</v>
       </c>
       <c r="AL4" s="1" t="s">
         <v>106</v>
@@ -2734,10 +2736,10 @@
         <v>108</v>
       </c>
       <c r="AS4" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="AT4" s="6" t="s">
         <v>271</v>
-      </c>
-      <c r="AT4" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="AU4" s="1" t="s">
         <v>109</v>
@@ -2755,10 +2757,10 @@
         <v>112</v>
       </c>
       <c r="BA4" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="BB4" s="19" t="s">
         <v>273</v>
-      </c>
-      <c r="BB4" s="20" t="s">
-        <v>274</v>
       </c>
       <c r="BC4" s="1" t="s">
         <v>113</v>
@@ -2781,20 +2783,20 @@
       <c r="BL4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BM4" s="1" t="s">
+      <c r="BM4" s="13" t="s">
         <v>115</v>
       </c>
       <c r="BN4" s="1">
         <v>30</v>
       </c>
-      <c r="BP4" s="1" t="s">
+      <c r="BP4" s="13" t="s">
         <v>89</v>
       </c>
       <c r="BQ4" s="1" t="s">
         <v>116</v>
       </c>
       <c r="BS4" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="BT4" s="1" t="s">
         <v>117</v>
@@ -2802,11 +2804,11 @@
       <c r="BU4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="BV4" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW4" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="BW4" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="BX4" s="5">
         <v>875784</v>
@@ -2818,7 +2820,7 @@
         <v>250</v>
       </c>
       <c r="CF4" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CG4" s="1" t="s">
         <v>121</v>
@@ -2829,7 +2831,7 @@
       <c r="CL4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="CM4" s="20">
+      <c r="CM4" s="19">
         <v>30</v>
       </c>
       <c r="CQ4" s="1" t="s">
@@ -2840,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="CS4" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="CT4" s="5">
         <f t="shared" si="1"/>
@@ -2869,10 +2871,10 @@
         <v>123</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>73</v>
@@ -2881,7 +2883,7 @@
         <v>124</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>125</v>
@@ -2896,7 +2898,7 @@
         <v>128</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q5" s="1" t="str">
         <f t="shared" si="2"/>
@@ -2905,17 +2907,17 @@
       <c r="R5" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="S5" s="1" t="b">
+      <c r="S5" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U5" s="1" t="s">
-        <v>243</v>
+      <c r="U5" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W5" s="8">
         <v>4.3899999999999997</v>
@@ -2927,7 +2929,7 @@
         <v>49</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>130</v>
@@ -2936,10 +2938,10 @@
         <v>81</v>
       </c>
       <c r="AI5" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AJ5" s="19" t="s">
         <v>279</v>
-      </c>
-      <c r="AJ5" s="20" t="s">
-        <v>280</v>
       </c>
       <c r="AO5" s="1" t="s">
         <v>132</v>
@@ -2951,10 +2953,10 @@
         <v>133</v>
       </c>
       <c r="AS5" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="AT5" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="AT5" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="AV5" s="1" t="s">
         <v>131</v>
@@ -2965,9 +2967,9 @@
       <c r="AX5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BA5" s="29"/>
-      <c r="BB5" s="30"/>
-      <c r="BC5" s="29"/>
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="29"/>
+      <c r="BC5" s="28"/>
       <c r="BD5" s="1" t="s">
         <v>79</v>
       </c>
@@ -2988,13 +2990,13 @@
       <c r="BL5" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="BM5" s="1" t="s">
+      <c r="BM5" s="13" t="s">
         <v>115</v>
       </c>
       <c r="BO5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="BP5" s="1" t="s">
+      <c r="BP5" s="13" t="s">
         <v>89</v>
       </c>
       <c r="BQ5" s="1" t="s">
@@ -3004,7 +3006,7 @@
         <v>138</v>
       </c>
       <c r="BS5" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="BT5" s="1" t="s">
         <v>117</v>
@@ -3012,11 +3014,11 @@
       <c r="BU5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BV5" s="1" t="s">
+      <c r="BV5" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW5" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="BW5" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="BX5" s="5">
         <v>4185236</v>
@@ -3028,7 +3030,7 @@
         <v>75</v>
       </c>
       <c r="CF5" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CG5" s="1" t="s">
         <v>143</v>
@@ -3039,7 +3041,7 @@
       <c r="CL5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="CM5" s="20">
+      <c r="CM5" s="19">
         <v>30</v>
       </c>
       <c r="CP5" s="1" t="s">
@@ -3053,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="CS5" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="CT5" s="5">
         <f t="shared" si="1"/>
@@ -3082,10 +3084,10 @@
         <v>145</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>73</v>
@@ -3109,7 +3111,7 @@
         <v>151</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q6" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3118,17 +3120,17 @@
       <c r="R6" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="S6" s="1" t="b">
+      <c r="S6" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U6" s="1" t="s">
-        <v>243</v>
+      <c r="U6" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W6" s="8">
         <v>61</v>
@@ -3140,7 +3142,7 @@
         <v>49</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>153</v>
@@ -3149,10 +3151,10 @@
         <v>81</v>
       </c>
       <c r="AI6" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="AJ6" s="19" t="s">
         <v>283</v>
-      </c>
-      <c r="AJ6" s="20" t="s">
-        <v>284</v>
       </c>
       <c r="AL6" s="1" t="s">
         <v>154</v>
@@ -3167,10 +3169,10 @@
         <v>155</v>
       </c>
       <c r="AS6" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="AT6" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="AT6" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="AU6" s="1" t="s">
         <v>156</v>
@@ -3191,10 +3193,10 @@
         <v>160</v>
       </c>
       <c r="BA6" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="BB6" s="19" t="s">
         <v>287</v>
-      </c>
-      <c r="BB6" s="20" t="s">
-        <v>288</v>
       </c>
       <c r="BD6" s="1" t="s">
         <v>79</v>
@@ -3219,17 +3221,17 @@
       <c r="BL6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="BM6" s="1" t="s">
+      <c r="BM6" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="BP6" s="1" t="s">
+      <c r="BP6" s="13" t="s">
         <v>89</v>
       </c>
       <c r="BQ6" s="1" t="s">
         <v>163</v>
       </c>
       <c r="BS6" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="BT6" s="1" t="s">
         <v>117</v>
@@ -3237,11 +3239,11 @@
       <c r="BU6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BV6" s="1" t="s">
+      <c r="BV6" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW6" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="BW6" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="BX6" s="5">
         <v>1787205</v>
@@ -3256,7 +3258,7 @@
         <v>149</v>
       </c>
       <c r="CF6" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CG6" s="1" t="s">
         <v>166</v>
@@ -3264,7 +3266,7 @@
       <c r="CK6" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="CM6" s="20">
+      <c r="CM6" s="19">
         <v>30</v>
       </c>
       <c r="CP6" s="1" t="s">
@@ -3278,7 +3280,7 @@
         <v>1</v>
       </c>
       <c r="CS6" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="CT6" s="5">
         <f t="shared" si="1"/>
@@ -3307,10 +3309,10 @@
         <v>168</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>73</v>
@@ -3334,7 +3336,7 @@
         <v>174</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q7" s="1" t="str">
         <f t="shared" si="2"/>
@@ -3343,17 +3345,17 @@
       <c r="R7" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="S7" s="1" t="b">
+      <c r="S7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="U7" s="1" t="s">
-        <v>243</v>
+      <c r="U7" s="13" t="s">
+        <v>242</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W7" s="8">
         <v>65</v>
@@ -3365,7 +3367,7 @@
         <v>49</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>153</v>
@@ -3374,10 +3376,10 @@
         <v>81</v>
       </c>
       <c r="AI7" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="AJ7" s="19" t="s">
         <v>291</v>
-      </c>
-      <c r="AJ7" s="20" t="s">
-        <v>292</v>
       </c>
       <c r="AL7" s="1" t="s">
         <v>177</v>
@@ -3392,10 +3394,10 @@
         <v>179</v>
       </c>
       <c r="AS7" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="AT7" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="AT7" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="AU7" s="1" t="s">
         <v>180</v>
@@ -3413,13 +3415,13 @@
         <v>182</v>
       </c>
       <c r="BA7" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="BB7" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="BB7" s="20" t="s">
-        <v>288</v>
-      </c>
       <c r="BC7" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="BD7" s="1" t="s">
         <v>79</v>
@@ -3441,13 +3443,13 @@
       <c r="BL7" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BM7" s="1" t="s">
+      <c r="BM7" s="13" t="s">
         <v>88</v>
       </c>
       <c r="BO7" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="BP7" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="BP7" s="13" t="s">
         <v>89</v>
       </c>
       <c r="BQ7" s="1" t="s">
@@ -3457,7 +3459,7 @@
         <v>185</v>
       </c>
       <c r="BS7" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="BT7" s="1" t="s">
         <v>117</v>
@@ -3465,11 +3467,11 @@
       <c r="BU7" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BV7" s="1" t="s">
+      <c r="BV7" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="BW7" s="13" t="s">
         <v>252</v>
-      </c>
-      <c r="BW7" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="BX7" s="5">
         <v>2187622</v>
@@ -3481,7 +3483,7 @@
         <v>250</v>
       </c>
       <c r="CF7" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="CG7" s="1" t="s">
         <v>188</v>
@@ -3492,7 +3494,7 @@
       <c r="CL7" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="CM7" s="20"/>
+      <c r="CM7" s="19"/>
       <c r="CP7" s="1" t="s">
         <v>187</v>
       </c>
@@ -3504,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="CS7" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="CT7" s="5">
         <f t="shared" si="1"/>
@@ -3518,607 +3520,607 @@
       </c>
     </row>
     <row r="8" spans="1:100" s="1" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="H8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="I8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="O8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="P8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q8" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="R8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="S8" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="T8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="U8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="V8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="W8" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="X8" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="Z8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="I8" s="26" t="s">
+      <c r="AA8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AB8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AC8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AD8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AF8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AG8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AH8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AI8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="AJ8" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="AK8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AL8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AM8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AN8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AO8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AP8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AQ8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AR8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AS8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="AT8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="AU8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AV8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AW8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AX8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AY8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="AZ8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BA8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="N8" s="26" t="s">
+      <c r="BB8" s="27" t="s">
         <v>298</v>
       </c>
-      <c r="O8" s="26" t="s">
+      <c r="BC8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BD8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="P8" s="26" t="s">
+      <c r="BE8" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="Q8" s="26" t="s">
+      <c r="BF8" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="R8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="S8" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="T8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="U8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="V8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="W8" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="X8" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="Z8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="AA8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AB8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AC8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AD8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AE8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AF8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AG8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AH8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AI8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="AJ8" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="AK8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AL8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AM8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AN8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AO8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AP8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AQ8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AR8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AS8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="AT8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="AU8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AV8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AW8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AX8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AY8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="AZ8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BA8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="BB8" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="BC8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BD8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="BE8" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="BF8" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="BG8" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="BH8" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="BI8" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="BJ8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BK8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BL8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BM8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BN8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BO8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BP8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BQ8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BR8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BS8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BT8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BU8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BV8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BW8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BX8" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="BY8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="BZ8" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="CA8" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="CB8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CC8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CD8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CE8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CF8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CG8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CH8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CI8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CJ8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CK8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CL8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CM8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CN8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CO8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CP8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CQ8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CR8" s="26" t="s">
-        <v>301</v>
-      </c>
-      <c r="CS8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CT8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CU8" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="CV8" s="26" t="s">
-        <v>298</v>
+      <c r="BG8" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="BH8" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="BI8" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="BJ8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BK8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BL8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BM8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BN8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BO8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BP8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BQ8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BR8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BS8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BT8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BU8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BV8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BW8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BX8" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="BY8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="BZ8" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="CA8" s="25" t="s">
+        <v>296</v>
+      </c>
+      <c r="CB8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CC8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CD8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CE8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CF8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CG8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CH8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CI8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CJ8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CK8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CL8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CM8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CN8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CO8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CP8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CQ8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CR8" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="CS8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CT8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CU8" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="CV8" s="25" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:100" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>406</v>
-      </c>
-      <c r="B9" s="31" t="s">
+      <c r="A9" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>303</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>304</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>305</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="F9" s="30" t="s">
         <v>306</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="G9" s="30" t="s">
         <v>307</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="H9" s="30" t="s">
         <v>308</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="I9" s="30" t="s">
         <v>309</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="J9" s="30" t="s">
         <v>310</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="K9" s="30" t="s">
         <v>311</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="L9" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="M9" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="N9" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="O9" s="30" t="s">
         <v>315</v>
       </c>
-      <c r="O9" s="31" t="s">
+      <c r="P9" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="Q9" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="Q9" s="31" t="s">
+      <c r="R9" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="R9" s="31" t="s">
+      <c r="S9" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="S9" s="31" t="s">
+      <c r="T9" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="T9" s="31" t="s">
+      <c r="U9" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="U9" s="31" t="s">
+      <c r="V9" s="30" t="s">
         <v>322</v>
       </c>
-      <c r="V9" s="31" t="s">
+      <c r="W9" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="W9" s="31" t="s">
+      <c r="X9" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="X9" s="31" t="s">
+      <c r="Y9" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="Y9" s="31" t="s">
+      <c r="Z9" s="30" t="s">
         <v>326</v>
       </c>
-      <c r="Z9" s="31" t="s">
+      <c r="AA9" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="AA9" s="31" t="s">
+      <c r="AB9" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="AB9" s="31" t="s">
+      <c r="AC9" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="AC9" s="31" t="s">
+      <c r="AD9" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="AD9" s="31" t="s">
+      <c r="AE9" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="AE9" s="31" t="s">
+      <c r="AF9" s="30" t="s">
         <v>332</v>
       </c>
-      <c r="AF9" s="31" t="s">
+      <c r="AG9" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="AG9" s="31" t="s">
+      <c r="AH9" s="30" t="s">
         <v>334</v>
       </c>
-      <c r="AH9" s="31" t="s">
+      <c r="AI9" s="30" t="s">
         <v>335</v>
       </c>
-      <c r="AI9" s="31" t="s">
+      <c r="AJ9" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="AJ9" s="31" t="s">
+      <c r="AK9" s="30" t="s">
         <v>337</v>
       </c>
-      <c r="AK9" s="31" t="s">
+      <c r="AL9" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="AL9" s="31" t="s">
+      <c r="AM9" s="30" t="s">
         <v>339</v>
       </c>
-      <c r="AM9" s="31" t="s">
+      <c r="AN9" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="AN9" s="31" t="s">
+      <c r="AO9" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="AO9" s="31" t="s">
+      <c r="AP9" s="30" t="s">
         <v>342</v>
       </c>
-      <c r="AP9" s="31" t="s">
+      <c r="AQ9" s="30" t="s">
         <v>343</v>
       </c>
-      <c r="AQ9" s="31" t="s">
+      <c r="AR9" s="30" t="s">
         <v>344</v>
       </c>
-      <c r="AR9" s="31" t="s">
+      <c r="AS9" s="30" t="s">
         <v>345</v>
       </c>
-      <c r="AS9" s="31" t="s">
+      <c r="AT9" s="30" t="s">
         <v>346</v>
       </c>
-      <c r="AT9" s="31" t="s">
+      <c r="AU9" s="30" t="s">
         <v>347</v>
       </c>
-      <c r="AU9" s="31" t="s">
+      <c r="AV9" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="AV9" s="31" t="s">
+      <c r="AW9" s="30" t="s">
         <v>349</v>
       </c>
-      <c r="AW9" s="31" t="s">
+      <c r="AX9" s="30" t="s">
         <v>350</v>
       </c>
-      <c r="AX9" s="31" t="s">
+      <c r="AY9" s="30" t="s">
         <v>351</v>
       </c>
-      <c r="AY9" s="31" t="s">
+      <c r="AZ9" s="30" t="s">
         <v>352</v>
       </c>
-      <c r="AZ9" s="31" t="s">
+      <c r="BA9" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="BA9" s="31" t="s">
+      <c r="BB9" s="30" t="s">
         <v>354</v>
       </c>
-      <c r="BB9" s="31" t="s">
+      <c r="BC9" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="BC9" s="31" t="s">
+      <c r="BD9" s="30" t="s">
         <v>356</v>
       </c>
-      <c r="BD9" s="31" t="s">
+      <c r="BE9" s="30" t="s">
         <v>357</v>
       </c>
-      <c r="BE9" s="31" t="s">
+      <c r="BF9" s="30" t="s">
         <v>358</v>
       </c>
-      <c r="BF9" s="31" t="s">
+      <c r="BG9" s="30" t="s">
         <v>359</v>
       </c>
-      <c r="BG9" s="31" t="s">
+      <c r="BH9" s="30" t="s">
         <v>360</v>
       </c>
-      <c r="BH9" s="31" t="s">
+      <c r="BI9" s="30" t="s">
         <v>361</v>
       </c>
-      <c r="BI9" s="31" t="s">
+      <c r="BJ9" s="30" t="s">
         <v>362</v>
       </c>
-      <c r="BJ9" s="31" t="s">
+      <c r="BK9" s="30" t="s">
         <v>363</v>
       </c>
-      <c r="BK9" s="31" t="s">
+      <c r="BL9" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="BL9" s="31" t="s">
+      <c r="BM9" s="30" t="s">
         <v>365</v>
       </c>
-      <c r="BM9" s="31" t="s">
+      <c r="BN9" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="BN9" s="31" t="s">
+      <c r="BO9" s="30" t="s">
         <v>367</v>
       </c>
-      <c r="BO9" s="31" t="s">
+      <c r="BP9" s="30" t="s">
         <v>368</v>
       </c>
-      <c r="BP9" s="31" t="s">
+      <c r="BQ9" s="30" t="s">
         <v>369</v>
       </c>
-      <c r="BQ9" s="31" t="s">
+      <c r="BR9" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="BR9" s="31" t="s">
+      <c r="BS9" s="30" t="s">
         <v>371</v>
       </c>
-      <c r="BS9" s="31" t="s">
+      <c r="BT9" s="30" t="s">
         <v>372</v>
       </c>
-      <c r="BT9" s="31" t="s">
+      <c r="BU9" s="30" t="s">
         <v>373</v>
       </c>
-      <c r="BU9" s="31" t="s">
+      <c r="BV9" s="30" t="s">
         <v>374</v>
       </c>
-      <c r="BV9" s="31" t="s">
+      <c r="BW9" s="30" t="s">
         <v>375</v>
       </c>
-      <c r="BW9" s="31" t="s">
+      <c r="BX9" s="30" t="s">
         <v>376</v>
       </c>
-      <c r="BX9" s="31" t="s">
+      <c r="BY9" s="30" t="s">
         <v>377</v>
       </c>
-      <c r="BY9" s="31" t="s">
+      <c r="BZ9" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="CA9" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="CB9" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="CC9" s="30" t="s">
         <v>378</v>
       </c>
-      <c r="BZ9" s="31" t="s">
+      <c r="CD9" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="CE9" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="CF9" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="CG9" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="CH9" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="CI9" s="30" t="s">
         <v>386</v>
       </c>
-      <c r="CA9" s="31" t="s">
+      <c r="CJ9" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="CK9" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="CL9" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="CM9" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="CN9" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="CO9" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="CP9" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="CQ9" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="CR9" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="CS9" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="CT9" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="CU9" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="CB9" s="31" t="s">
-        <v>380</v>
-      </c>
-      <c r="CC9" s="31" t="s">
-        <v>379</v>
-      </c>
-      <c r="CD9" s="31" t="s">
-        <v>381</v>
-      </c>
-      <c r="CE9" s="31" t="s">
-        <v>382</v>
-      </c>
-      <c r="CF9" s="31" t="s">
-        <v>383</v>
-      </c>
-      <c r="CG9" s="31" t="s">
-        <v>384</v>
-      </c>
-      <c r="CH9" s="31" t="s">
-        <v>385</v>
-      </c>
-      <c r="CI9" s="31" t="s">
-        <v>387</v>
-      </c>
-      <c r="CJ9" s="31" t="s">
-        <v>388</v>
-      </c>
-      <c r="CK9" s="31" t="s">
-        <v>392</v>
-      </c>
-      <c r="CL9" s="31" t="s">
-        <v>393</v>
-      </c>
-      <c r="CM9" s="31" t="s">
-        <v>394</v>
-      </c>
-      <c r="CN9" s="31" t="s">
-        <v>395</v>
-      </c>
-      <c r="CO9" s="31" t="s">
-        <v>396</v>
-      </c>
-      <c r="CP9" s="31" t="s">
-        <v>397</v>
-      </c>
-      <c r="CQ9" s="31" t="s">
+      <c r="CV9" s="30" t="s">
         <v>398</v>
-      </c>
-      <c r="CR9" s="31" t="s">
-        <v>391</v>
-      </c>
-      <c r="CS9" s="31" t="s">
-        <v>401</v>
-      </c>
-      <c r="CT9" s="31" t="s">
-        <v>402</v>
-      </c>
-      <c r="CU9" s="31" t="s">
-        <v>390</v>
-      </c>
-      <c r="CV9" s="31" t="s">
-        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>